<commit_message>
Extended canonical name assignment to pregrant data
</commit_message>
<xml_diff>
--- a/tests/post_processing/PVDI_11_Inventor_Canonical_Test_Cases.xlsx
+++ b/tests/post_processing/PVDI_11_Inventor_Canonical_Test_Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smadhavan/Universe/Projects/Current/PatentsView/Update Pipeline/PatentsView-DB/tests/post_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBEAAB9-1A19-2D4B-A52B-46DFA8686DA0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C8863A-197B-1144-B802-283CDC81E12E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="960" windowWidth="24020" windowHeight="14240" activeTab="2" xr2:uid="{D815E5C6-C656-2F41-8FF4-0E1DFE6D63CF}"/>
+    <workbookView xWindow="980" yWindow="920" windowWidth="24020" windowHeight="14240" xr2:uid="{D815E5C6-C656-2F41-8FF4-0E1DFE6D63CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiple_Names_Case" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>name_last</t>
   </si>
   <si>
-    <t>patent_date</t>
-  </si>
-  <si>
     <t>fl:a_ln:abbasi-5</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>final_name_last</t>
+  </si>
+  <si>
+    <t>doc_date</t>
   </si>
 </sst>
 </file>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEBFF79-FBFA-1E4C-B9AC-02A0B3CF8027}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -472,173 +472,173 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>39273</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>38559</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
         <v>37943</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>42633</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>38993</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1">
         <v>42906</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>38307</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1">
         <v>36613</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +651,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -673,33 +673,33 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>37852</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735EFE2B-8691-9447-8F78-0C2845F05F2C}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -728,93 +728,93 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="1">
         <v>36095</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>37026</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1">
         <v>41023</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>41891</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>